<commit_message>
Fundamental Version 2 Release
</commit_message>
<xml_diff>
--- a/Fundamentals/fundamentals_test_cases.xlsx
+++ b/Fundamentals/fundamentals_test_cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SENECA COURSES CPP\CPR101NII\Final Group Project\Project Source Code_Lathesan_Vadivelu\Fundamentals\Fundamentals.ver.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SENECA COURSES CPP\CPR101NII\Final Group Project\Project Source Code_Lathesan_Vadivelu\Fundamentals\Fundamentals.Ver.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB588922-7C9A-49E0-9F38-CF6E96C8150F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BA96DE8-E4B7-45D6-B1BF-81C13FC289B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="60">
   <si>
     <t>Program
 or module:</t>
@@ -455,6 +455,68 @@
   </si>
   <si>
     <t>Hello</t>
+  </si>
+  <si>
+    <r>
+      <t>(POSITIVE TEST CASE[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>➕</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">])  
+------------------------------------
+Type a string (q - to quit):
+</t>
+    </r>
+  </si>
+  <si>
+    <t>theotherside</t>
+  </si>
+  <si>
+    <t>The length is 12</t>
+  </si>
+  <si>
+    <t>The code counted the amount of characters in the string and ouputted the length of the string.</t>
+  </si>
+  <si>
+    <t>s (258 times)</t>
+  </si>
+  <si>
+    <t>The length is 258</t>
+  </si>
+  <si>
+    <t>it is able to handle nubers that range in the hundreds, this was expected. not testing any higher.</t>
+  </si>
+  <si>
+    <t>Entered nothing, only pressed the enter key</t>
+  </si>
+  <si>
+    <t>The length is 0</t>
+  </si>
+  <si>
+    <t>The program Ends when the character "q" is given, and moves onto the next demo/module</t>
+  </si>
+  <si>
+    <t>*** Start of Measuring Strings Demo ***</t>
+  </si>
+  <si>
+    <t>Can take nothing and still give 0 as character length</t>
+  </si>
+  <si>
+    <t>Lathesan Vadivelu
+April 08, 2022</t>
   </si>
 </sst>
 </file>
@@ -1294,8 +1356,8 @@
   </sheetPr>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1570,7 +1632,7 @@
         <v>2</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="12" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1597,65 +1659,151 @@
       </c>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="21"/>
-      <c r="I15" s="29"/>
-    </row>
-    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="21"/>
-      <c r="I16" s="29"/>
-    </row>
-    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="21"/>
-      <c r="I17" s="29"/>
-    </row>
-    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="21"/>
-      <c r="I18" s="29"/>
-    </row>
-    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="21"/>
-      <c r="I19" s="31"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="30"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="21"/>
-      <c r="I20" s="31"/>
+    <row r="15" spans="1:9" s="56" customFormat="1" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="51" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="54"/>
+      <c r="I15" s="55"/>
+    </row>
+    <row r="16" spans="1:9" s="56" customFormat="1" ht="157.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="54"/>
+      <c r="I16" s="55"/>
+    </row>
+    <row r="17" spans="1:9" s="47" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A17" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="59" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="46"/>
+    </row>
+    <row r="18" spans="1:9" s="47" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A18" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="I18" s="46"/>
+    </row>
+    <row r="19" spans="1:9" s="47" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A19" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="57" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" s="46"/>
+    </row>
+    <row r="20" spans="1:9" s="47" customFormat="1" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="I20" s="46"/>
     </row>
     <row r="21" spans="1:9" s="12" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="60" t="s">

</xml_diff>